<commit_message>
Successfully wrote excel file.
</commit_message>
<xml_diff>
--- a/tests/Unit/Roster/data/small_partly_filled.xlsx
+++ b/tests/Unit/Roster/data/small_partly_filled.xlsx
@@ -3067,10 +3067,10 @@
   <dimension ref="A2:AS603"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
@@ -3394,7 +3394,9 @@
       </c>
       <c r="I10" s="36"/>
       <c r="J10" s="37"/>
-      <c r="K10" s="36"/>
+      <c r="K10" s="36" t="n">
+        <v>0</v>
+      </c>
       <c r="L10" s="38"/>
       <c r="M10" s="35"/>
       <c r="N10" s="35"/>
@@ -3423,11 +3425,11 @@
       <c r="AK10" s="41"/>
       <c r="AL10" s="42" t="n">
         <f aca="false">COUNTIF(F100:AK101, "&gt;1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM10" s="43" t="n">
         <f aca="false">SUM(F100:AK101)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="AN10" s="44" t="n">
         <f aca="false">AO10*3.7</f>
@@ -3453,7 +3455,9 @@
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="51"/>
-      <c r="K11" s="50"/>
+      <c r="K11" s="50" t="n">
+        <v>0.333333333333333</v>
+      </c>
       <c r="L11" s="52"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
@@ -7231,7 +7235,7 @@
       </c>
       <c r="K100" s="151" t="n">
         <f aca="false">MOD(K11-K10, 1)*24</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L100" s="151" t="n">
         <f aca="false">MOD(L11-L10, 1)*24</f>
@@ -30050,7 +30054,7 @@
       <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30073,7 +30077,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30096,7 +30100,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30119,7 +30123,7 @@
       <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="161" width="8"/>
@@ -40820,7 +40824,7 @@
       <c r="B123" s="355"/>
       <c r="C123" s="371" t="n">
         <f aca="true">NOW()</f>
-        <v>45468.5694176078</v>
+        <v>45469.4361803897</v>
       </c>
       <c r="D123" s="371"/>
       <c r="E123" s="355"/>
@@ -41435,7 +41439,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="2" style="0" width="5.01"/>
@@ -41557,9 +41561,9 @@
         <f aca="false">IF('Darbo grafikas'!J9&lt;&gt;"",IF('Darbo grafikas'!J10&lt;&gt;"",IF('Darbo grafikas'!J9='Darbo grafikas'!J10,"",IF('Darbo grafikas'!J9&lt;'Darbo grafikas'!J10,('Darbo grafikas'!J10-'Darbo grafikas'!J9)*24,('Darbo grafikas'!J10-'Darbo grafikas'!J9+1)*24)),""),"")</f>
         <v/>
       </c>
-      <c r="F2" s="373" t="str">
+      <c r="F2" s="373" t="n">
         <f aca="false">IF('Darbo grafikas'!K9&lt;&gt;"",IF('Darbo grafikas'!K10&lt;&gt;"",IF('Darbo grafikas'!K9='Darbo grafikas'!K10,"",IF('Darbo grafikas'!K9&lt;'Darbo grafikas'!K10,('Darbo grafikas'!K10-'Darbo grafikas'!K9)*24,('Darbo grafikas'!K10-'Darbo grafikas'!K9+1)*24)),""),"")</f>
-        <v/>
+        <v>-120</v>
       </c>
       <c r="G2" s="373" t="str">
         <f aca="false">IF('Darbo grafikas'!L9&lt;&gt;"",IF('Darbo grafikas'!L10&lt;&gt;"",IF('Darbo grafikas'!L9='Darbo grafikas'!L10,"",IF('Darbo grafikas'!L9&lt;'Darbo grafikas'!L10,('Darbo grafikas'!L10-'Darbo grafikas'!L9)*24,('Darbo grafikas'!L10-'Darbo grafikas'!L9+1)*24)),""),"")</f>
@@ -41683,9 +41687,9 @@
         <f aca="false">IF('Darbo grafikas'!J10&lt;&gt;"",IF('Darbo grafikas'!J11&lt;&gt;"",IF('Darbo grafikas'!J10='Darbo grafikas'!J11,"",IF('Darbo grafikas'!J10&lt;'Darbo grafikas'!J11,('Darbo grafikas'!J11-'Darbo grafikas'!J10)*24,('Darbo grafikas'!J11-'Darbo grafikas'!J10+1)*24)),""),"")</f>
         <v/>
       </c>
-      <c r="F3" s="373" t="str">
+      <c r="F3" s="373" t="n">
         <f aca="false">IF('Darbo grafikas'!K10&lt;&gt;"",IF('Darbo grafikas'!K11&lt;&gt;"",IF('Darbo grafikas'!K10='Darbo grafikas'!K11,"",IF('Darbo grafikas'!K10&lt;'Darbo grafikas'!K11,('Darbo grafikas'!K11-'Darbo grafikas'!K10)*24,('Darbo grafikas'!K11-'Darbo grafikas'!K10+1)*24)),""),"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G3" s="373" t="str">
         <f aca="false">IF('Darbo grafikas'!L10&lt;&gt;"",IF('Darbo grafikas'!L11&lt;&gt;"",IF('Darbo grafikas'!L10='Darbo grafikas'!L11,"",IF('Darbo grafikas'!L10&lt;'Darbo grafikas'!L11,('Darbo grafikas'!L11-'Darbo grafikas'!L10)*24,('Darbo grafikas'!L11-'Darbo grafikas'!L10+1)*24)),""),"")</f>
@@ -45464,7 +45468,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="149"/>

</xml_diff>